<commit_message>
Update Personal Finance Project.xlsx
</commit_message>
<xml_diff>
--- a/Personal Finance Project.xlsx
+++ b/Personal Finance Project.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6fbf94b95efba8fc/Desktop/Python Stuff/CSE_111/final_project/cse111_final_project/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="192" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5870E60-2D42-4A91-BDA8-0EA8C21556A8}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="3072" windowWidth="17496" windowHeight="8880" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -97,7 +102,7 @@
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,18 +485,18 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29.25">
+    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -534,7 +539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -554,7 +559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -574,7 +579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -604,16 +609,16 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -621,7 +626,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="29.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -630,7 +635,7 @@
         <v>4950</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -639,7 +644,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
reading has been fixed
</commit_message>
<xml_diff>
--- a/Personal Finance Project.xlsx
+++ b/Personal Finance Project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6fbf94b95efba8fc/Desktop/Python Stuff/CSE_111/final_project/cse111_final_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\BYUI Collage classes\2025 Winter\cse111_final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="192" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5870E60-2D42-4A91-BDA8-0EA8C21556A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB50C3B-A975-4BBF-A68C-27DB81A52DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="3072" windowWidth="17496" windowHeight="8880" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -482,7 +482,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,9 +608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DB4C27-E7D4-46E4-9D4A-47B2BAF5227C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>